<commit_message>
Center login form vertically and horizontally using flexbox
</commit_message>
<xml_diff>
--- a/disabled_students_report.xlsx
+++ b/disabled_students_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,22 +496,94 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Administrator</t>
+          <t>Dennis</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>cdddd</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>images.jpg</t>
-        </is>
-      </c>
+          <t>ddddd</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-22 12:32:07</t>
+          <t>2025-05-25 15:07:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Aliasgar bhai Mulla Shabbir bhai Semari Wala</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>28527</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2 B M</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Dennis</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dddd</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>SBoys print25043012510.jpg</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-05-25 15:07:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Aliasgar bhai Mulla Shabbir bhai Semari Wala</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>28527</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2 B M</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mellisa</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ewwewe</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-05-25 15:13:53</t>
         </is>
       </c>
     </row>

</xml_diff>